<commit_message>
fix v-for của data.js 17:40 25/03/21
</commit_message>
<xml_diff>
--- a/eShop-fncTest-VTT.xlsx
+++ b/eShop-fncTest-VTT.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Màn hình chính" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="182">
   <si>
     <t>UI</t>
   </si>
@@ -597,6 +597,30 @@
   </si>
   <si>
     <t>Bản ghi ấy không hiển thị lên trang chủ nữa</t>
+  </si>
+  <si>
+    <t>Hiển thị chữ</t>
+  </si>
+  <si>
+    <t>Chữ căn trái</t>
+  </si>
+  <si>
+    <t>Hiển thị số</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Số căn phải, giá tiền có chấm </t>
+  </si>
+  <si>
+    <t>Nhập tối đa 20 ký tự</t>
+  </si>
+  <si>
+    <t>Hiển thị giá tiền</t>
+  </si>
+  <si>
+    <t>Giá tiền có chấm, căn phải</t>
+  </si>
+  <si>
+    <t>Nhập tối đa được 20 ký tự</t>
   </si>
 </sst>
 </file>
@@ -939,10 +963,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F35"/>
+  <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1005,73 +1029,75 @@
         <v>6</v>
       </c>
     </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
+      <c r="B7" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
         <v>2</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B8" s="2" t="s">
         <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
-        <v>113</v>
+        <v>7</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>114</v>
+        <v>8</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B11" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C11" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E11" s="2" t="s">
         <v>102</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="B11" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
-        <v>107</v>
+        <v>9</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>108</v>
+        <v>11</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>109</v>
+        <v>12</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>104</v>
@@ -1080,40 +1106,43 @@
         <v>101</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B14" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C14" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="E14" s="2" t="s">
         <v>106</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B14" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
-        <v>110</v>
+        <v>13</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>111</v>
+        <v>15</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>112</v>
+        <v>12</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>16</v>
@@ -1121,55 +1150,55 @@
     </row>
     <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
-        <v>17</v>
+        <v>110</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>18</v>
+        <v>111</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>112</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
         <v>17</v>
       </c>
       <c r="C17" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B18" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D18" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="E18" s="2" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B18" s="2" t="s">
+    <row r="19" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B19" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C19" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="E18" s="2" t="s">
+      <c r="E19" s="2" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B19" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
         <v>20</v>
       </c>
@@ -1177,46 +1206,49 @@
         <v>119</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="2" t="s">
         <v>20</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>22</v>
+        <v>119</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>28</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="s">
         <v>20</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="2" t="s">
         <v>20</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>120</v>
+        <v>24</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" s="2" t="s">
         <v>20</v>
       </c>
@@ -1224,133 +1256,144 @@
         <v>120</v>
       </c>
       <c r="E24" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B25" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="E25" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B25" s="2" t="s">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B26" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B26" s="2" t="s">
-        <v>33</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>31</v>
       </c>
       <c r="D26" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B27" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D27" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E26" s="2" t="s">
+      <c r="E27" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B27" s="2" t="s">
+    <row r="28" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B28" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C28" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D27" s="2">
+      <c r="D28" s="2">
         <v>25</v>
       </c>
-      <c r="E27" s="2" t="s">
+      <c r="E28" s="2" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="B28" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B29" s="2" t="s">
         <v>81</v>
       </c>
       <c r="C29" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="B30" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C30" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="D29" s="2" t="s">
+      <c r="D30" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="E29" s="2" t="s">
+      <c r="E30" s="2" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="B30" s="2" t="s">
+    <row r="31" spans="2:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="B31" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="C31" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="D30" s="2" t="s">
+      <c r="D31" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="E30" s="2" t="s">
+      <c r="E31" s="2" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B31" s="2" t="s">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B32" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="C32" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="E31" s="2" t="s">
+      <c r="E32" s="2" t="s">
         <v>92</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="2">
-        <v>3</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
+        <v>3</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="2">
         <v>4</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B34" s="2" t="s">
         <v>41</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="C34" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="C35" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="C36" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E35" s="2" t="s">
+      <c r="E36" s="2" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1364,8 +1407,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1410,6 +1453,17 @@
         <v>47</v>
       </c>
     </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B3" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>2</v>
@@ -1460,7 +1514,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>54</v>
       </c>
@@ -1595,7 +1649,7 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1609,7 +1663,7 @@
     <col min="7" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" ht="37.5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>97</v>
       </c>
@@ -1635,6 +1689,17 @@
       </c>
       <c r="B2" s="2" t="s">
         <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B3" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1776,7 +1841,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>

</xml_diff>